<commit_message>
Info for new PDF pages
</commit_message>
<xml_diff>
--- a/data/info_for_pdf.xlsx
+++ b/data/info_for_pdf.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codyclifford/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmolenaar/Desktop/BROGAARD/Gaard/Gaard Reporting System/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6210D0B3-536C-6347-BD8B-468489F73428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B843D1-D1C3-E244-9E5E-1AB7665A7B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15760" xr2:uid="{6D522E3E-A00D-E248-87E0-EF62B3A29ADA}"/>
+    <workbookView xWindow="-53760" yWindow="-8360" windowWidth="46780" windowHeight="17940" xr2:uid="{6D522E3E-A00D-E248-87E0-EF62B3A29ADA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B2519F-DAD7-424B-BCCD-A6F236E5C7A3}">
   <dimension ref="B3:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F17" sqref="F1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated Firm Name cell
</commit_message>
<xml_diff>
--- a/data/info_for_pdf.xlsx
+++ b/data/info_for_pdf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmolenaar/Desktop/BROGAARD/Gaard/Gaard Reporting System/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C2D87A-6004-3A42-BED8-BAA93E3B14A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4118B0-9B8D-794A-8CFD-A303DFF88244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-53760" yWindow="-8360" windowWidth="46780" windowHeight="17940" xr2:uid="{6D522E3E-A00D-E248-87E0-EF62B3A29ADA}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="41120" windowHeight="25800" xr2:uid="{6D522E3E-A00D-E248-87E0-EF62B3A29ADA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>Gaard Capital Quarterly Portfolio Report</t>
-  </si>
-  <si>
-    <t>Gaard Capital, LLC</t>
-  </si>
-  <si>
     <t>Brogaard Asset Protection Trust</t>
   </si>
   <si>
@@ -192,6 +186,12 @@
   </si>
   <si>
     <t>Treasury yields edged lower once again in March, despite Federal Reserve officials holding the overnight rate steady for the second straight FOMC meeting. The overriding theme of the quarter was the Trump tariffs, more specifically the uncertainty fueled by the on-again/off-again series of threats aimed primarily at U.S. neighbors to the north and south. Those threats became reality on March 3rd when a 25% tax was imposed on goods imported from Mexico and Canada, while an additional 10% tax was placed on Chinese imports, doubling the previously imposed 10%. Two days later, Trump decided that Mexican and Canadian goods falling under the USMCA agreement he negotiated five years earlier would be exempt. The following day, tariffs on Canadian dairy products and lumber were announced, followed by a 25% tax on all steel and aluminum imported into the United States. This seemingly random pattern repeated itself throughout the month, shaking consumer and business confidence. Trade partners quickly retaliated by levying new tariffs and increasing existing duties on U.S. goods. Perhaps more importantly, foreign countries scrambled to forge new agreements among themselves, reducing barriers to promote free trade. Stocks experienced a particularly volatile month, during which the S&amp;P 500 lost nearly 6%, despite corporate profits reaching an all-time high in the prior quarter. Initial concerns over tariff-related inflation increasingly morphed into recession fears. Extreme uncertainty likely stalled business investment and consumer spending. Very few economic releases in March reflected the rapidly evolving tariff situation, making the data less useful as a predictor of future activity, although still helpful in establishing a baseline. Overall, employment held up well, inflation generally moved lower, and consumer spending weakened. Nonfarm payrolls for February were roughly in line with forecasts at an acceptable +151,000, while the unemployment rate ticked up from 4.0% to 4.1%, still very near historical lows. Both the overall CPI index and core CPI rose 0.2% in February, a tenth below the 0.3% median forecasts. On a year-over-year basis, headline CPI declined from 3.0% to 2.8%, and core CPI decreased to 3.1%, which, although still elevated, marked a four-year low. Highly visible grocery prices were unchanged, and gas prices were slightly lower. Headline retail sales, expected to rebound from a weak January, rose just 0.2% in February, well below the 0.6% median forecast, while the previously reported January decline was revised lower from -0.9% to -1.2%. Weakness was broad-based, with 7 of 13 spending categories declining. Tariff concerns were more evident in soft data, as survey results deteriorated sharply. The Conference Board’s main consumer confidence index for March fell 7.2 points to 92.9, while expectations for the next six months dropped nearly 10 points to 65.2, the lowest level in 12 years and consistent with an economic downturn. Pessimism regarding future business conditions and employment prospects increased significantly, while inflation expectations rose to 6.2% over the next 12 months. The University of Michigan consumer sentiment survey reported long-term inflation expectations reaching a three-decade high. As expected, the Federal Reserve held rates steady at the March FOMC meeting. Updated economic projections showed slightly higher inflation and lower GDP growth for 2025. The dot plot continued to indicate two rate cuts in 2025, although with less conviction than in December. Chair Powell’s view that tariff-related inflation would be temporary suggested policymakers could cut rates sooner and more aggressively if the labor market and broader economy weakened, even if inflation moved higher, provided tariffs were the primary driver of price increases. Although a near-term recession remains unlikely, the Atlanta Fed’s GDPNow estimate for Q1 stood at -3.7% as of April 1st. This figure will likely improve as March data are incorporated, but it nonetheless reflects an abrupt and potentially severe first-quarter slowdown. With few positive catalysts expected in the second quarter, particularly if global trade tensions intensify, financial markets are likely to continue bracing for economic weakness and lower interest rates.</t>
+  </si>
+  <si>
+    <t>Quarterly Portfolio Report</t>
+  </si>
+  <si>
+    <t>Gaard Capital LLC</t>
   </si>
 </sst>
 </file>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B2519F-DAD7-424B-BCCD-A6F236E5C7A3}">
   <dimension ref="B3:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,31 +593,31 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <v>46050</v>
@@ -625,31 +625,31 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>0.24</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>0.46</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>0.35</v>
@@ -673,15 +673,15 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>0.1</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>0.2</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>0.15</v>
@@ -705,15 +705,15 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>7.0000000000000007E-2</v>
@@ -729,7 +729,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26">
         <v>0.05</v>
@@ -737,15 +737,15 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29">
         <v>0.55000000000000004</v>
@@ -753,15 +753,15 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -769,7 +769,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>0.11</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>0.05</v>
@@ -785,15 +785,15 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C39">
         <v>0.04</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C40">
         <v>0.2</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C41">
         <v>0.1</v>
@@ -817,15 +817,15 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C44">
         <v>0.2</v>
@@ -833,15 +833,15 @@
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C48">
         <v>0.27</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C49">
         <v>0.2</v>
@@ -865,15 +865,15 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C53">
         <v>0.1</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C54">
         <v>0.05</v>
@@ -897,26 +897,26 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C57" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C59" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Market Recap Verbal
</commit_message>
<xml_diff>
--- a/data/info_for_pdf.xlsx
+++ b/data/info_for_pdf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmolenaar/Desktop/BROGAARD/Gaard/Gaard Reporting System/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4118B0-9B8D-794A-8CFD-A303DFF88244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BE5B13-B7EE-094B-93F1-C246E967077E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="41120" windowHeight="25800" xr2:uid="{6D522E3E-A00D-E248-87E0-EF62B3A29ADA}"/>
   </bookViews>
@@ -185,13 +185,18 @@
     <t>Gaard Capital, LLC (“Gaard”), a registered investment advisor. This material is intended to provide general information about the market, Gaard and its services. The views expressed in the referenced materials are subject to change based on market and other conditions. These documents may contain certain statements that may be deemed forward-looking statements. Please note that any such statements are not guarantees of any future performance and actual results or developments may differ materially from those projected. Any projections, market outlooks, or estimates are based upon certain assumptions and should not be construed as indicative of actual events that will occur. This material is being provided to you upon your request and is for informational purposes only. The information provided herein does not constitute investment advice and is not a solicitation to buy or sell securities. Market data, articles, and other content in this material are based on generally available information and are believed to be reliable. Gaard does not guarantee the accuracy of the information contained in this material. The information is of a general nature and should not be construed as investment advice. While we use reasonable efforts to furnish accurate and up-to-date information, we do not warrant that any information contained in or made available through this material is accurate, complete, reliable, current, or error-free. We assume no liability or responsibility for any errors or omissions in the content of these materials or other communications. Any information presented about tax considerations affecting client financial transactions or arrangements is not intended as tax advice and should not be relied upon for the purpose of avoiding any tax penalties. Gaard does not provide tax, accounting, or legal advice. This material was not intended or written to be used, and it cannot be used by any taxpayer, for the purpose of avoiding penalties that may be imposed on the taxpayer under U.S. federal tax laws. The information provided is for educational and informational purposes only and does not constitute investment advice, and it should not be relied on as such. It should not be considered a solicitation to buy or an offer to sell a security. It does not take into account any investor's particular investment objectives, strategies, tax status, or investment horizon. You should consult your attorney or tax advisor.</t>
   </si>
   <si>
-    <t>Treasury yields edged lower once again in March, despite Federal Reserve officials holding the overnight rate steady for the second straight FOMC meeting. The overriding theme of the quarter was the Trump tariffs, more specifically the uncertainty fueled by the on-again/off-again series of threats aimed primarily at U.S. neighbors to the north and south. Those threats became reality on March 3rd when a 25% tax was imposed on goods imported from Mexico and Canada, while an additional 10% tax was placed on Chinese imports, doubling the previously imposed 10%. Two days later, Trump decided that Mexican and Canadian goods falling under the USMCA agreement he negotiated five years earlier would be exempt. The following day, tariffs on Canadian dairy products and lumber were announced, followed by a 25% tax on all steel and aluminum imported into the United States. This seemingly random pattern repeated itself throughout the month, shaking consumer and business confidence. Trade partners quickly retaliated by levying new tariffs and increasing existing duties on U.S. goods. Perhaps more importantly, foreign countries scrambled to forge new agreements among themselves, reducing barriers to promote free trade. Stocks experienced a particularly volatile month, during which the S&amp;P 500 lost nearly 6%, despite corporate profits reaching an all-time high in the prior quarter. Initial concerns over tariff-related inflation increasingly morphed into recession fears. Extreme uncertainty likely stalled business investment and consumer spending. Very few economic releases in March reflected the rapidly evolving tariff situation, making the data less useful as a predictor of future activity, although still helpful in establishing a baseline. Overall, employment held up well, inflation generally moved lower, and consumer spending weakened. Nonfarm payrolls for February were roughly in line with forecasts at an acceptable +151,000, while the unemployment rate ticked up from 4.0% to 4.1%, still very near historical lows. Both the overall CPI index and core CPI rose 0.2% in February, a tenth below the 0.3% median forecasts. On a year-over-year basis, headline CPI declined from 3.0% to 2.8%, and core CPI decreased to 3.1%, which, although still elevated, marked a four-year low. Highly visible grocery prices were unchanged, and gas prices were slightly lower. Headline retail sales, expected to rebound from a weak January, rose just 0.2% in February, well below the 0.6% median forecast, while the previously reported January decline was revised lower from -0.9% to -1.2%. Weakness was broad-based, with 7 of 13 spending categories declining. Tariff concerns were more evident in soft data, as survey results deteriorated sharply. The Conference Board’s main consumer confidence index for March fell 7.2 points to 92.9, while expectations for the next six months dropped nearly 10 points to 65.2, the lowest level in 12 years and consistent with an economic downturn. Pessimism regarding future business conditions and employment prospects increased significantly, while inflation expectations rose to 6.2% over the next 12 months. The University of Michigan consumer sentiment survey reported long-term inflation expectations reaching a three-decade high. As expected, the Federal Reserve held rates steady at the March FOMC meeting. Updated economic projections showed slightly higher inflation and lower GDP growth for 2025. The dot plot continued to indicate two rate cuts in 2025, although with less conviction than in December. Chair Powell’s view that tariff-related inflation would be temporary suggested policymakers could cut rates sooner and more aggressively if the labor market and broader economy weakened, even if inflation moved higher, provided tariffs were the primary driver of price increases. Although a near-term recession remains unlikely, the Atlanta Fed’s GDPNow estimate for Q1 stood at -3.7% as of April 1st. This figure will likely improve as March data are incorporated, but it nonetheless reflects an abrupt and potentially severe first-quarter slowdown. With few positive catalysts expected in the second quarter, particularly if global trade tensions intensify, financial markets are likely to continue bracing for economic weakness and lower interest rates.</t>
-  </si>
-  <si>
     <t>Quarterly Portfolio Report</t>
   </si>
   <si>
     <t>Gaard Capital LLC</t>
+  </si>
+  <si>
+    <t>Treasury yields moved lower again in March even as the Federal Reserve held its policy rate steady for the second consecutive FOMC meeting. The dominant theme of the quarter was uncertainty surrounding President Trump’s tariff policy, characterized by rapidly changing announcements and reversals. On March 3, a 25% tariff was imposed on imports from Mexico and Canada, along with an additional 10% tariff on Chinese goods. Within days, exemptions were granted for USMCA-covered goods, while new tariffs were announced on Canadian dairy and lumber, followed by a 25% levy on all imported steel and aluminum. Retaliation from trade partners was swift, and several countries sought new trade agreements among themselves, increasing global trade fragmentation.
+Markets reacted negatively to this uncertainty. Stocks were highly volatile, and the S&amp;P 500 fell nearly 6% in March despite record corporate profits in the prior quarter. Investor concerns shifted from tariff-driven inflation to fears of an economic slowdown or recession, as heightened uncertainty likely weighed on business investment and consumer spending.
+Hard economic data still reflected pre-tariff conditions and therefore provided limited insight into future activity. Employment remained solid, with February nonfarm payrolls rising 151,000 and the unemployment rate edging up to 4.1%, still near historic lows. Inflation eased modestly: both headline and core CPI rose 0.2% in February, below expectations, with year-over-year headline inflation falling to 2.8% and core CPI to 3.1%, a four-year low. Grocery prices were flat and gasoline prices declined slightly.
+Consumer spending showed clear weakness. February retail sales rose only 0.2%, well below forecasts, while January sales were revised down to a 1.2% decline. Spending fell in 7 of 13 categories. Softer survey data reflected growing concern: the Conference Board consumer confidence index dropped sharply in March, and expectations fell to a 12-year low consistent with recessionary conditions. Inflation expectations rose, a trend reinforced by the University of Michigan sentiment survey, which showed long-term inflation expectations at a three-decade high.
+At its March meeting, the Federal Reserve left rates unchanged and revised projections to show slightly higher inflation and lower 2025 GDP growth. The dot plot still signaled two rate cuts in 2025, though with reduced confidence. Chair Powell emphasized that tariff-driven inflation would likely be temporary, suggesting policymakers could ease policy if economic or labor market conditions deteriorated.
+While a near-term recession remains uncertain, the Atlanta Fed GDPNow estimate pointed to a sharp Q1 contraction of -3.7% as of April 1. Although this estimate may improve with additional data, it underscores a sudden slowdown. With few positive catalysts expected in the second quarter and trade tensions still elevated, financial markets appear increasingly positioned for slower growth and lower interest rates.</t>
   </si>
 </sst>
 </file>
@@ -234,10 +239,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B2519F-DAD7-424B-BCCD-A6F236E5C7A3}">
   <dimension ref="B3:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,7 +602,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
@@ -604,7 +610,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
@@ -907,8 +913,8 @@
       <c r="B57" t="s">
         <v>34</v>
       </c>
-      <c r="C57" t="s">
-        <v>49</v>
+      <c r="C57" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added in Quarter key/value
</commit_message>
<xml_diff>
--- a/data/info_for_pdf.xlsx
+++ b/data/info_for_pdf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmolenaar/Desktop/BROGAARD/Gaard/Gaard Reporting System/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6BE5B13-B7EE-094B-93F1-C246E967077E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E245BF-E627-DD40-B510-4E73CA28FECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="41120" windowHeight="25800" xr2:uid="{6D522E3E-A00D-E248-87E0-EF62B3A29ADA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>key</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Gaard Capital logo handled in report template</t>
   </si>
   <si>
-    <t>The purpose of the endowment is to generate income and long-term appreciation that will be expended according to donor- or Board-approved purposes and spending policy for each endowment. The goal of the Organization’s investment program is to achieve a 5 percent nominal total return, net of all management and custodial fees. This target represents the long-term performance needed to support the Organization’s mission by funding annual spending requirements, covering inflation, and maintaining the purchasing power of invested assets.</t>
-  </si>
-  <si>
     <t>page_1_report_title</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>page_4_ips_non_us_equity_em_target</t>
   </si>
   <si>
-    <t>page_4_ips_total_equities_target</t>
-  </si>
-  <si>
     <t>page_4_ips_non_us_fixed_income_global_range_min</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
   </si>
   <si>
     <t>page_4_non_us_equity_em_current</t>
-  </si>
-  <si>
-    <t>page_4_total_equities_current</t>
   </si>
   <si>
     <t>page_4_non_us_fixed_income_global_current</t>
@@ -197,6 +188,15 @@
 Consumer spending showed clear weakness. February retail sales rose only 0.2%, well below forecasts, while January sales were revised down to a 1.2% decline. Spending fell in 7 of 13 categories. Softer survey data reflected growing concern: the Conference Board consumer confidence index dropped sharply in March, and expectations fell to a 12-year low consistent with recessionary conditions. Inflation expectations rose, a trend reinforced by the University of Michigan sentiment survey, which showed long-term inflation expectations at a three-decade high.
 At its March meeting, the Federal Reserve left rates unchanged and revised projections to show slightly higher inflation and lower 2025 GDP growth. The dot plot still signaled two rate cuts in 2025, though with reduced confidence. Chair Powell emphasized that tariff-driven inflation would likely be temporary, suggesting policymakers could ease policy if economic or labor market conditions deteriorated.
 While a near-term recession remains uncertain, the Atlanta Fed GDPNow estimate pointed to a sharp Q1 contraction of -3.7% as of April 1. Although this estimate may improve with additional data, it underscores a sudden slowdown. With few positive catalysts expected in the second quarter and trade tensions still elevated, financial markets appear increasingly positioned for slower growth and lower interest rates.</t>
+  </si>
+  <si>
+    <t>The purpose of the endowment is to generate income and long-term appreciation that will be expended according to donor- or Board-approved purposes and spending policy for each endowment. The goal of the Organization’s investment program is to achieve a 5% nominal total return, net of all management and custodial fees. This target represents the long-term performance needed to support the Organization’s mission by funding annual spending requirements, covering inflation, and maintaining the purchasing power of invested assets.</t>
+  </si>
+  <si>
+    <t>quarter</t>
+  </si>
+  <si>
+    <t>Q1</t>
   </si>
 </sst>
 </file>
@@ -239,11 +239,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B2519F-DAD7-424B-BCCD-A6F236E5C7A3}">
-  <dimension ref="B3:C59"/>
+  <dimension ref="B3:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,170 +598,178 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1">
-        <v>46050</v>
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>46050</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14">
-        <v>0.24</v>
+      <c r="C13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>0.46</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16">
-        <v>0.35</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
-        <v>0.1</v>
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
+      <c r="C23" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29">
-        <v>0.55000000000000004</v>
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" t="s">
-        <v>38</v>
+        <v>19</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>0.11</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.2">
@@ -770,31 +777,31 @@
         <v>21</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>22</v>
       </c>
-      <c r="C33">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+      <c r="C37">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>23</v>
       </c>
-      <c r="C34">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" t="s">
-        <v>38</v>
+      <c r="C38">
+        <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.2">
@@ -802,47 +809,47 @@
         <v>24</v>
       </c>
       <c r="C39">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41">
-        <v>0.1</v>
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44">
+        <v>25</v>
+      </c>
+      <c r="C42">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" t="s">
-        <v>38</v>
+        <v>26</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46">
+        <v>0.27</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.2">
@@ -850,31 +857,31 @@
         <v>28</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49">
-        <v>0.2</v>
+        <v>43</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" t="s">
-        <v>38</v>
+        <v>29</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51">
+        <v>0.1</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.2">
@@ -882,47 +889,31 @@
         <v>31</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>33</v>
-      </c>
-      <c r="C54">
-        <v>0.05</v>
+        <v>44</v>
+      </c>
+      <c r="C53" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" t="s">
         <v>34</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved: Since Inception correct %. Updated Quarter Return Headers, Updated Risk Header: now Since Inception
</commit_message>
<xml_diff>
--- a/data/info_for_pdf.xlsx
+++ b/data/info_for_pdf.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10222"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelmolenaar/Desktop/BROGAARD/Gaard/Gaard Reporting System/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E245BF-E627-DD40-B510-4E73CA28FECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BF861B-7D05-714F-8514-17E2571A53AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="41120" windowHeight="25800" xr2:uid="{6D522E3E-A00D-E248-87E0-EF62B3A29ADA}"/>
   </bookViews>
@@ -196,7 +196,7 @@
     <t>quarter</t>
   </si>
   <si>
-    <t>Q1</t>
+    <t>Q4</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="B3:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>